<commit_message>
db to already commented videos
</commit_message>
<xml_diff>
--- a/axis-y.xlsx
+++ b/axis-y.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/armanlyosman/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/armanlyosman/PycharmProjects/CommentatorV2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EBAC318-EC6E-0041-9F8A-95B4F4A0E50E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2B42DB6D-BB45-A54B-8093-90399A2C0DC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="320" yWindow="660" windowWidth="24940" windowHeight="14760" xr2:uid="{6B154F5E-0F15-EE47-8317-EFE35FAB9579}"/>
   </bookViews>

</xml_diff>

<commit_message>
fix response by templates and add tem,plate words
</commit_message>
<xml_diff>
--- a/axis-y.xlsx
+++ b/axis-y.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/armanlyosman/PycharmProjects/CommentatorV2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2B42DB6D-BB45-A54B-8093-90399A2C0DC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68FF3BBB-CA96-C441-AF7B-56B4DB3F3A2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="320" yWindow="660" windowWidth="24940" windowHeight="14760" xr2:uid="{6B154F5E-0F15-EE47-8317-EFE35FAB9579}"/>
   </bookViews>
@@ -38,9 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
-    <t>0u0p4m4U</t>
-  </si>
-  <si>
     <t>mrBreakfast</t>
   </si>
   <si>
@@ -69,16 +66,28 @@
   </si>
   <si>
     <t>Комментарий</t>
+  </si>
+  <si>
+    <t>0u0p4M4u@!</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <charset val="204"/>
@@ -102,16 +111,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -447,7 +461,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -458,10 +472,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
         <v>9</v>
-      </c>
-      <c r="B1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -469,44 +483,47 @@
         <v>476283763</v>
       </c>
       <c r="B2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1" xr:uid="{C3CAC427-E40E-0148-BED9-EABD8B8B3CF9}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>